<commit_message>
filter added, length changed
</commit_message>
<xml_diff>
--- a/data/ire odi matches.xlsx
+++ b/data/ire odi matches.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgallagher/repos/bootstrap-react-treetable-tester/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D239C1AC-93E8-594A-BB3A-DA36FD40D592}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A185DE2F-FEA5-0445-AB60-4E10342E9153}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ire odi matches" sheetId="1" r:id="rId1"/>
     <sheet name="json" sheetId="2" r:id="rId2"/>
+    <sheet name="ire odi matches by ground" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="2937" uniqueCount="176">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="3687" uniqueCount="176">
   <si>
     <t>Team</t>
   </si>
@@ -568,9 +569,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1052,7 +1053,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1407,7 +1408,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6112,10 +6113,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K65" sqref="K65"/>
     </sheetView>
   </sheetViews>
@@ -15142,4 +15143,4709 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A18646-F04C-D346-935E-738F22ADFC8B}">
+  <dimension ref="A1:I164"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>112</v>
+      </c>
+      <c r="C2">
+        <v>28.4</v>
+      </c>
+      <c r="D2">
+        <v>3.9</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>156</v>
+      </c>
+      <c r="H2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="2" t="d">
+        <v>2008-07-01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>4.2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I3" s="2" t="d">
+        <v>2008-07-02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>114</v>
+      </c>
+      <c r="I4" s="2" t="d">
+        <v>2009-08-22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+      <c r="D5">
+        <v>5.38</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" t="s">
+        <v>157</v>
+      </c>
+      <c r="I5" s="2" t="d">
+        <v>2021-01-08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>237</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>4.74</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" t="s">
+        <v>88</v>
+      </c>
+      <c r="I6" s="2" t="d">
+        <v>2015-03-15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7">
+        <v>39.1</v>
+      </c>
+      <c r="D7">
+        <v>3.95</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="2" t="d">
+        <v>2010-07-07</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <v>5.36</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="2" t="d">
+        <v>2013-07-09</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>236</v>
+      </c>
+      <c r="C9">
+        <v>49.5</v>
+      </c>
+      <c r="D9">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="2" t="d">
+        <v>2013-07-07</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>177</v>
+      </c>
+      <c r="C10">
+        <v>48.2</v>
+      </c>
+      <c r="D10">
+        <v>3.66</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="2" t="d">
+        <v>2010-07-09</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11">
+        <v>44.5</v>
+      </c>
+      <c r="D11">
+        <v>5.19</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="2" t="d">
+        <v>2010-07-10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>274</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
+      </c>
+      <c r="D12">
+        <v>5.48</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="2" t="d">
+        <v>2006-08-08</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13">
+        <v>50</v>
+      </c>
+      <c r="D13">
+        <v>4.8</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="2" t="d">
+        <v>2006-08-05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14">
+        <v>50</v>
+      </c>
+      <c r="D14">
+        <v>5.3</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" t="s">
+        <v>65</v>
+      </c>
+      <c r="I14" s="2" t="d">
+        <v>2016-07-19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15">
+        <v>47.3</v>
+      </c>
+      <c r="D15">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" s="2" t="d">
+        <v>2016-07-14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>211</v>
+      </c>
+      <c r="C16">
+        <v>48.2</v>
+      </c>
+      <c r="D16">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" t="s">
+        <v>65</v>
+      </c>
+      <c r="I16" s="2" t="d">
+        <v>2016-07-12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>210</v>
+      </c>
+      <c r="C17">
+        <v>48.5</v>
+      </c>
+      <c r="D17">
+        <v>4.3</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" s="2" t="d">
+        <v>2019-05-19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <v>198</v>
+      </c>
+      <c r="C18">
+        <v>48.3</v>
+      </c>
+      <c r="D18">
+        <v>4.08</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" t="s">
+        <v>65</v>
+      </c>
+      <c r="I18" s="2" t="d">
+        <v>2018-08-27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C19">
+        <v>43.5</v>
+      </c>
+      <c r="D19">
+        <v>4.17</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19" t="s">
+        <v>65</v>
+      </c>
+      <c r="I19" s="2" t="d">
+        <v>2018-08-29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20">
+        <v>179</v>
+      </c>
+      <c r="C20">
+        <v>41.2</v>
+      </c>
+      <c r="D20">
+        <v>4.33</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" t="s">
+        <v>65</v>
+      </c>
+      <c r="I20" s="2" t="d">
+        <v>2019-05-21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>150</v>
+      </c>
+      <c r="C21">
+        <v>41</v>
+      </c>
+      <c r="D21">
+        <v>3.65</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" t="s">
+        <v>65</v>
+      </c>
+      <c r="I21" s="2" t="d">
+        <v>2016-07-17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22">
+        <v>124</v>
+      </c>
+      <c r="C22">
+        <v>36.1</v>
+      </c>
+      <c r="D22">
+        <v>3.42</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" t="s">
+        <v>65</v>
+      </c>
+      <c r="I22" s="2" t="d">
+        <v>2018-08-31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23">
+        <v>157</v>
+      </c>
+      <c r="C23">
+        <v>23.4</v>
+      </c>
+      <c r="D23">
+        <v>6.63</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" t="s">
+        <v>120</v>
+      </c>
+      <c r="H23" t="s">
+        <v>65</v>
+      </c>
+      <c r="I23" s="2" t="d">
+        <v>2015-08-27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" t="s">
+        <v>149</v>
+      </c>
+      <c r="C24">
+        <v>10.4</v>
+      </c>
+      <c r="D24">
+        <v>3.37</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G24" t="s">
+        <v>120</v>
+      </c>
+      <c r="H24" t="s">
+        <v>65</v>
+      </c>
+      <c r="I24" s="2" t="d">
+        <v>2012-06-23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25">
+        <v>45</v>
+      </c>
+      <c r="D25">
+        <v>5.22</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" t="s">
+        <v>42</v>
+      </c>
+      <c r="H25" t="s">
+        <v>65</v>
+      </c>
+      <c r="I25" s="2" t="d">
+        <v>2010-07-15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26">
+        <v>46</v>
+      </c>
+      <c r="D26">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" t="s">
+        <v>42</v>
+      </c>
+      <c r="H26" t="s">
+        <v>65</v>
+      </c>
+      <c r="I26" s="2" t="d">
+        <v>2010-07-16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27">
+        <v>50</v>
+      </c>
+      <c r="D27">
+        <v>5.26</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" t="s">
+        <v>65</v>
+      </c>
+      <c r="I27" s="2" t="d">
+        <v>2006-06-13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28">
+        <v>20</v>
+      </c>
+      <c r="D28">
+        <v>5.6</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I28" s="2" t="d">
+        <v>2009-08-27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29">
+        <v>193</v>
+      </c>
+      <c r="C29">
+        <v>50</v>
+      </c>
+      <c r="D29">
+        <v>3.86</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H29" t="s">
+        <v>65</v>
+      </c>
+      <c r="I29" s="2" t="d">
+        <v>2007-06-23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" t="s">
+        <v>137</v>
+      </c>
+      <c r="C30">
+        <v>50</v>
+      </c>
+      <c r="D30">
+        <v>2.96</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" t="s">
+        <v>44</v>
+      </c>
+      <c r="H30" t="s">
+        <v>65</v>
+      </c>
+      <c r="I30" s="2" t="d">
+        <v>2008-08-24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="1" t="d">
+        <v>2021-02-18</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+      <c r="D31">
+        <v>2.25</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>55</v>
+      </c>
+      <c r="G31" t="s">
+        <v>44</v>
+      </c>
+      <c r="H31" t="s">
+        <v>65</v>
+      </c>
+      <c r="I31" s="2" t="d">
+        <v>2008-08-25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32">
+        <v>50</v>
+      </c>
+      <c r="D32">
+        <v>4.2</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" t="s">
+        <v>35</v>
+      </c>
+      <c r="H32" t="s">
+        <v>65</v>
+      </c>
+      <c r="I32" s="2" t="d">
+        <v>2007-07-11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33">
+        <v>50</v>
+      </c>
+      <c r="D33">
+        <v>4.76</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>25</v>
+      </c>
+      <c r="G33" t="s">
+        <v>54</v>
+      </c>
+      <c r="H33" t="s">
+        <v>65</v>
+      </c>
+      <c r="I33" s="2" t="d">
+        <v>2011-05-30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34">
+        <v>96</v>
+      </c>
+      <c r="C34">
+        <v>20</v>
+      </c>
+      <c r="D34">
+        <v>4.8</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" t="s">
+        <v>54</v>
+      </c>
+      <c r="H34" t="s">
+        <v>65</v>
+      </c>
+      <c r="I34" s="2" t="d">
+        <v>2011-05-28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35">
+        <v>49.5</v>
+      </c>
+      <c r="D35">
+        <v>4.51</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" t="s">
+        <v>65</v>
+      </c>
+      <c r="I35" s="2" t="d">
+        <v>2013-09-06</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36">
+        <v>50</v>
+      </c>
+      <c r="D36">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" t="s">
+        <v>65</v>
+      </c>
+      <c r="I36" s="2" t="d">
+        <v>2007-07-15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" t="s">
+        <v>133</v>
+      </c>
+      <c r="C37">
+        <v>33</v>
+      </c>
+      <c r="D37">
+        <v>5.03</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" t="s">
+        <v>65</v>
+      </c>
+      <c r="I37" s="2" t="d">
+        <v>2013-09-08</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38">
+        <v>131</v>
+      </c>
+      <c r="C38">
+        <v>30.5</v>
+      </c>
+      <c r="D38">
+        <v>4.24</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G38" t="s">
+        <v>155</v>
+      </c>
+      <c r="H38" t="s">
+        <v>65</v>
+      </c>
+      <c r="I38" s="2" t="d">
+        <v>2007-06-24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39">
+        <v>50</v>
+      </c>
+      <c r="D39">
+        <v>4.84</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" t="s">
+        <v>65</v>
+      </c>
+      <c r="I39" s="2" t="d">
+        <v>2019-07-04</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" t="s">
+        <v>121</v>
+      </c>
+      <c r="C40">
+        <v>41.2</v>
+      </c>
+      <c r="D40">
+        <v>4.62</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" t="s">
+        <v>12</v>
+      </c>
+      <c r="H40" t="s">
+        <v>65</v>
+      </c>
+      <c r="I40" s="2" t="d">
+        <v>2019-07-07</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41">
+        <v>49.1</v>
+      </c>
+      <c r="D41">
+        <v>6.69</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" t="s">
+        <v>17</v>
+      </c>
+      <c r="H41" t="s">
+        <v>18</v>
+      </c>
+      <c r="I41" s="2" t="d">
+        <v>2011-03-02</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42">
+        <v>207</v>
+      </c>
+      <c r="C42">
+        <v>47.5</v>
+      </c>
+      <c r="D42">
+        <v>4.32</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42" t="s">
+        <v>25</v>
+      </c>
+      <c r="G42" t="s">
+        <v>70</v>
+      </c>
+      <c r="H42" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" s="2" t="d">
+        <v>2011-03-06</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43">
+        <v>198</v>
+      </c>
+      <c r="C43">
+        <v>43.5</v>
+      </c>
+      <c r="D43">
+        <v>4.51</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43" t="s">
+        <v>25</v>
+      </c>
+      <c r="G43" t="s">
+        <v>120</v>
+      </c>
+      <c r="H43" t="s">
+        <v>94</v>
+      </c>
+      <c r="I43" s="2" t="d">
+        <v>2016-09-27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44">
+        <v>41</v>
+      </c>
+      <c r="D44">
+        <v>5.43</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" t="s">
+        <v>22</v>
+      </c>
+      <c r="H44" t="s">
+        <v>94</v>
+      </c>
+      <c r="I44" s="2" t="d">
+        <v>2009-04-06</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45">
+        <v>37.4</v>
+      </c>
+      <c r="D45">
+        <v>6.18</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="F45" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" t="s">
+        <v>94</v>
+      </c>
+      <c r="I45" s="2" t="d">
+        <v>2009-04-01</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46">
+        <v>148</v>
+      </c>
+      <c r="C46">
+        <v>30.5</v>
+      </c>
+      <c r="D46">
+        <v>4.8</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46" t="s">
+        <v>25</v>
+      </c>
+      <c r="G46" t="s">
+        <v>155</v>
+      </c>
+      <c r="H46" t="s">
+        <v>94</v>
+      </c>
+      <c r="I46" s="2" t="d">
+        <v>2016-09-25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" t="s">
+        <v>72</v>
+      </c>
+      <c r="C47">
+        <v>48.3</v>
+      </c>
+      <c r="D47">
+        <v>5.31</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" t="s">
+        <v>73</v>
+      </c>
+      <c r="I47" s="2" t="d">
+        <v>2019-07-01</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48">
+        <v>91</v>
+      </c>
+      <c r="C48">
+        <v>30</v>
+      </c>
+      <c r="D48">
+        <v>3.03</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>25</v>
+      </c>
+      <c r="G48" t="s">
+        <v>120</v>
+      </c>
+      <c r="H48" t="s">
+        <v>78</v>
+      </c>
+      <c r="I48" s="2" t="d">
+        <v>2007-04-13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" t="s">
+        <v>77</v>
+      </c>
+      <c r="C49">
+        <v>50</v>
+      </c>
+      <c r="D49">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" t="s">
+        <v>11</v>
+      </c>
+      <c r="G49" t="s">
+        <v>42</v>
+      </c>
+      <c r="H49" t="s">
+        <v>78</v>
+      </c>
+      <c r="I49" s="2" t="d">
+        <v>2007-04-15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50">
+        <v>50</v>
+      </c>
+      <c r="D50">
+        <v>4.74</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" t="s">
+        <v>25</v>
+      </c>
+      <c r="G50" t="s">
+        <v>152</v>
+      </c>
+      <c r="H50" t="s">
+        <v>78</v>
+      </c>
+      <c r="I50" s="2" t="d">
+        <v>2020-01-09</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51">
+        <v>180</v>
+      </c>
+      <c r="C51">
+        <v>46.1</v>
+      </c>
+      <c r="D51">
+        <v>3.89</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" t="s">
+        <v>25</v>
+      </c>
+      <c r="G51" t="s">
+        <v>152</v>
+      </c>
+      <c r="H51" t="s">
+        <v>78</v>
+      </c>
+      <c r="I51" s="2" t="d">
+        <v>2020-01-07</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" t="s">
+        <v>47</v>
+      </c>
+      <c r="C52">
+        <v>49.2</v>
+      </c>
+      <c r="D52">
+        <v>5.65</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" t="s">
+        <v>31</v>
+      </c>
+      <c r="H52" t="s">
+        <v>48</v>
+      </c>
+      <c r="I52" s="2" t="d">
+        <v>2015-02-25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53">
+        <v>126</v>
+      </c>
+      <c r="C53">
+        <v>33</v>
+      </c>
+      <c r="D53">
+        <v>3.81</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" t="s">
+        <v>25</v>
+      </c>
+      <c r="G53" t="s">
+        <v>17</v>
+      </c>
+      <c r="H53" t="s">
+        <v>142</v>
+      </c>
+      <c r="I53" s="2" t="d">
+        <v>2017-05-05</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54">
+        <v>210</v>
+      </c>
+      <c r="C54">
+        <v>45</v>
+      </c>
+      <c r="D54">
+        <v>4.66</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="F54" t="s">
+        <v>25</v>
+      </c>
+      <c r="G54" t="s">
+        <v>155</v>
+      </c>
+      <c r="H54" t="s">
+        <v>115</v>
+      </c>
+      <c r="I54" s="2" t="d">
+        <v>2015-03-03</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" t="s">
+        <v>124</v>
+      </c>
+      <c r="C55">
+        <v>42.3</v>
+      </c>
+      <c r="D55">
+        <v>4.42</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="F55" t="s">
+        <v>11</v>
+      </c>
+      <c r="G55" t="s">
+        <v>22</v>
+      </c>
+      <c r="H55" t="s">
+        <v>125</v>
+      </c>
+      <c r="I55" s="2" t="d">
+        <v>2009-04-19</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>9</v>
+      </c>
+      <c r="B56" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56">
+        <v>49</v>
+      </c>
+      <c r="D56">
+        <v>5.3</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+      <c r="F56" t="s">
+        <v>11</v>
+      </c>
+      <c r="G56" t="s">
+        <v>39</v>
+      </c>
+      <c r="H56" t="s">
+        <v>69</v>
+      </c>
+      <c r="I56" s="2" t="d">
+        <v>2019-03-05</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57" t="s">
+        <v>108</v>
+      </c>
+      <c r="C57">
+        <v>47.2</v>
+      </c>
+      <c r="D57">
+        <v>4.62</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="F57" t="s">
+        <v>11</v>
+      </c>
+      <c r="G57" t="s">
+        <v>39</v>
+      </c>
+      <c r="H57" t="s">
+        <v>69</v>
+      </c>
+      <c r="I57" s="2" t="d">
+        <v>2019-03-10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>9</v>
+      </c>
+      <c r="B58">
+        <v>161</v>
+      </c>
+      <c r="C58">
+        <v>49.2</v>
+      </c>
+      <c r="D58">
+        <v>3.26</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58" t="s">
+        <v>25</v>
+      </c>
+      <c r="G58" t="s">
+        <v>39</v>
+      </c>
+      <c r="H58" t="s">
+        <v>69</v>
+      </c>
+      <c r="I58" s="2" t="d">
+        <v>2019-02-28</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59">
+        <v>114</v>
+      </c>
+      <c r="C59">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="D59">
+        <v>3.21</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+      <c r="F59" t="s">
+        <v>25</v>
+      </c>
+      <c r="G59" t="s">
+        <v>39</v>
+      </c>
+      <c r="H59" t="s">
+        <v>69</v>
+      </c>
+      <c r="I59" s="2" t="d">
+        <v>2019-03-08</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60" t="s">
+        <v>150</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60" t="s">
+        <v>151</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60" t="s">
+        <v>55</v>
+      </c>
+      <c r="G60" t="s">
+        <v>39</v>
+      </c>
+      <c r="H60" t="s">
+        <v>69</v>
+      </c>
+      <c r="I60" s="2" t="d">
+        <v>2019-03-02</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>9</v>
+      </c>
+      <c r="B61">
+        <v>214</v>
+      </c>
+      <c r="C61">
+        <v>45.3</v>
+      </c>
+      <c r="D61">
+        <v>4.7</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+      <c r="F61" t="s">
+        <v>25</v>
+      </c>
+      <c r="G61" t="s">
+        <v>42</v>
+      </c>
+      <c r="H61" t="s">
+        <v>111</v>
+      </c>
+      <c r="I61" s="2" t="d">
+        <v>2008-03-22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>9</v>
+      </c>
+      <c r="B62" t="s">
+        <v>126</v>
+      </c>
+      <c r="C62">
+        <v>50</v>
+      </c>
+      <c r="D62">
+        <v>3.7</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" t="s">
+        <v>25</v>
+      </c>
+      <c r="G62" t="s">
+        <v>42</v>
+      </c>
+      <c r="H62" t="s">
+        <v>111</v>
+      </c>
+      <c r="I62" s="2" t="d">
+        <v>2008-03-18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>9</v>
+      </c>
+      <c r="B63">
+        <v>178</v>
+      </c>
+      <c r="C63">
+        <v>45</v>
+      </c>
+      <c r="D63">
+        <v>3.95</v>
+      </c>
+      <c r="E63">
+        <v>2</v>
+      </c>
+      <c r="F63" t="s">
+        <v>25</v>
+      </c>
+      <c r="G63" t="s">
+        <v>42</v>
+      </c>
+      <c r="H63" t="s">
+        <v>111</v>
+      </c>
+      <c r="I63" s="2" t="d">
+        <v>2011-02-25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>9</v>
+      </c>
+      <c r="B64">
+        <v>162</v>
+      </c>
+      <c r="C64">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="D64">
+        <v>4.2</v>
+      </c>
+      <c r="E64">
+        <v>2</v>
+      </c>
+      <c r="F64" t="s">
+        <v>25</v>
+      </c>
+      <c r="G64" t="s">
+        <v>42</v>
+      </c>
+      <c r="H64" t="s">
+        <v>111</v>
+      </c>
+      <c r="I64" s="2" t="d">
+        <v>2008-03-20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>9</v>
+      </c>
+      <c r="B65" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65">
+        <v>43.2</v>
+      </c>
+      <c r="D65">
+        <v>4.17</v>
+      </c>
+      <c r="E65">
+        <v>2</v>
+      </c>
+      <c r="F65" t="s">
+        <v>11</v>
+      </c>
+      <c r="G65" t="s">
+        <v>39</v>
+      </c>
+      <c r="H65" t="s">
+        <v>158</v>
+      </c>
+      <c r="I65" s="2" t="d">
+        <v>2015-01-10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>9</v>
+      </c>
+      <c r="B66">
+        <v>175</v>
+      </c>
+      <c r="C66">
+        <v>43.3</v>
+      </c>
+      <c r="D66">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="E66">
+        <v>2</v>
+      </c>
+      <c r="F66" t="s">
+        <v>25</v>
+      </c>
+      <c r="G66" t="s">
+        <v>39</v>
+      </c>
+      <c r="H66" t="s">
+        <v>158</v>
+      </c>
+      <c r="I66" s="2" t="d">
+        <v>2015-01-17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67" t="s">
+        <v>106</v>
+      </c>
+      <c r="C67">
+        <v>46.3</v>
+      </c>
+      <c r="D67">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="E67">
+        <v>2</v>
+      </c>
+      <c r="F67" t="s">
+        <v>11</v>
+      </c>
+      <c r="G67" t="s">
+        <v>15</v>
+      </c>
+      <c r="H67" t="s">
+        <v>158</v>
+      </c>
+      <c r="I67" s="2" t="d">
+        <v>2015-01-12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>9</v>
+      </c>
+      <c r="B68">
+        <v>163</v>
+      </c>
+      <c r="C68">
+        <v>47</v>
+      </c>
+      <c r="D68">
+        <v>3.46</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68" t="s">
+        <v>11</v>
+      </c>
+      <c r="G68" t="s">
+        <v>39</v>
+      </c>
+      <c r="H68" t="s">
+        <v>23</v>
+      </c>
+      <c r="I68" s="2" t="d">
+        <v>2012-07-05</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>9</v>
+      </c>
+      <c r="B69">
+        <v>192</v>
+      </c>
+      <c r="C69">
+        <v>42</v>
+      </c>
+      <c r="D69">
+        <v>4.57</v>
+      </c>
+      <c r="E69">
+        <v>2</v>
+      </c>
+      <c r="F69" t="s">
+        <v>25</v>
+      </c>
+      <c r="G69" t="s">
+        <v>120</v>
+      </c>
+      <c r="H69" t="s">
+        <v>23</v>
+      </c>
+      <c r="I69" s="2" t="d">
+        <v>2010-06-17</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>9</v>
+      </c>
+      <c r="B70" t="s">
+        <v>41</v>
+      </c>
+      <c r="C70">
+        <v>50</v>
+      </c>
+      <c r="D70">
+        <v>5.84</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70" t="s">
+        <v>25</v>
+      </c>
+      <c r="G70" t="s">
+        <v>42</v>
+      </c>
+      <c r="H70" t="s">
+        <v>23</v>
+      </c>
+      <c r="I70" s="2" t="d">
+        <v>2019-05-15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>9</v>
+      </c>
+      <c r="B71" t="s">
+        <v>21</v>
+      </c>
+      <c r="C71">
+        <v>50</v>
+      </c>
+      <c r="D71">
+        <v>6.56</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71" t="s">
+        <v>11</v>
+      </c>
+      <c r="G71" t="s">
+        <v>22</v>
+      </c>
+      <c r="H71" t="s">
+        <v>23</v>
+      </c>
+      <c r="I71" s="2" t="d">
+        <v>2011-09-19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>9</v>
+      </c>
+      <c r="B72" t="s">
+        <v>76</v>
+      </c>
+      <c r="C72">
+        <v>50</v>
+      </c>
+      <c r="D72">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72" t="s">
+        <v>11</v>
+      </c>
+      <c r="G72" t="s">
+        <v>22</v>
+      </c>
+      <c r="H72" t="s">
+        <v>23</v>
+      </c>
+      <c r="I72" s="2" t="d">
+        <v>2011-09-20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>9</v>
+      </c>
+      <c r="B73" t="s">
+        <v>144</v>
+      </c>
+      <c r="C73">
+        <v>23</v>
+      </c>
+      <c r="D73">
+        <v>5.08</v>
+      </c>
+      <c r="E73">
+        <v>2</v>
+      </c>
+      <c r="F73" t="s">
+        <v>25</v>
+      </c>
+      <c r="G73" t="s">
+        <v>17</v>
+      </c>
+      <c r="H73" t="s">
+        <v>23</v>
+      </c>
+      <c r="I73" s="2" t="d">
+        <v>2011-08-25</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>9</v>
+      </c>
+      <c r="B74" t="s">
+        <v>74</v>
+      </c>
+      <c r="C74">
+        <v>50</v>
+      </c>
+      <c r="D74">
+        <v>5.12</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74" t="s">
+        <v>11</v>
+      </c>
+      <c r="G74" t="s">
+        <v>44</v>
+      </c>
+      <c r="H74" t="s">
+        <v>23</v>
+      </c>
+      <c r="I74" s="2" t="d">
+        <v>2009-07-12</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>9</v>
+      </c>
+      <c r="B75" t="s">
+        <v>110</v>
+      </c>
+      <c r="C75">
+        <v>48.5</v>
+      </c>
+      <c r="D75">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E75">
+        <v>2</v>
+      </c>
+      <c r="F75" t="s">
+        <v>11</v>
+      </c>
+      <c r="G75" t="s">
+        <v>44</v>
+      </c>
+      <c r="H75" t="s">
+        <v>23</v>
+      </c>
+      <c r="I75" s="2" t="d">
+        <v>2009-07-09</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>9</v>
+      </c>
+      <c r="B76" t="s">
+        <v>146</v>
+      </c>
+      <c r="C76">
+        <v>21</v>
+      </c>
+      <c r="D76">
+        <v>4.95</v>
+      </c>
+      <c r="E76">
+        <v>2</v>
+      </c>
+      <c r="F76" t="s">
+        <v>11</v>
+      </c>
+      <c r="G76" t="s">
+        <v>44</v>
+      </c>
+      <c r="H76" t="s">
+        <v>23</v>
+      </c>
+      <c r="I76" s="2" t="d">
+        <v>2009-07-11</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>9</v>
+      </c>
+      <c r="B77" t="s">
+        <v>51</v>
+      </c>
+      <c r="C77">
+        <v>50</v>
+      </c>
+      <c r="D77">
+        <v>5.5</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77" t="s">
+        <v>11</v>
+      </c>
+      <c r="G77" t="s">
+        <v>35</v>
+      </c>
+      <c r="H77" t="s">
+        <v>23</v>
+      </c>
+      <c r="I77" s="2" t="d">
+        <v>2010-08-16</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>9</v>
+      </c>
+      <c r="B78" t="s">
+        <v>138</v>
+      </c>
+      <c r="C78">
+        <v>29</v>
+      </c>
+      <c r="D78">
+        <v>4.93</v>
+      </c>
+      <c r="E78">
+        <v>2</v>
+      </c>
+      <c r="F78" t="s">
+        <v>11</v>
+      </c>
+      <c r="G78" t="s">
+        <v>35</v>
+      </c>
+      <c r="H78" t="s">
+        <v>23</v>
+      </c>
+      <c r="I78" s="2" t="d">
+        <v>2008-07-28</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>9</v>
+      </c>
+      <c r="B79" t="s">
+        <v>141</v>
+      </c>
+      <c r="C79">
+        <v>20.3</v>
+      </c>
+      <c r="D79">
+        <v>6.29</v>
+      </c>
+      <c r="E79">
+        <v>2</v>
+      </c>
+      <c r="F79" t="s">
+        <v>11</v>
+      </c>
+      <c r="G79" t="s">
+        <v>35</v>
+      </c>
+      <c r="H79" t="s">
+        <v>23</v>
+      </c>
+      <c r="I79" s="2" t="d">
+        <v>2010-08-18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>9</v>
+      </c>
+      <c r="B80">
+        <v>238</v>
+      </c>
+      <c r="C80">
+        <v>45.3</v>
+      </c>
+      <c r="D80">
+        <v>5.23</v>
+      </c>
+      <c r="E80">
+        <v>2</v>
+      </c>
+      <c r="F80" t="s">
+        <v>25</v>
+      </c>
+      <c r="G80" t="s">
+        <v>156</v>
+      </c>
+      <c r="H80" t="s">
+        <v>23</v>
+      </c>
+      <c r="I80" s="2" t="d">
+        <v>2017-05-14</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>9</v>
+      </c>
+      <c r="B81">
+        <v>154</v>
+      </c>
+      <c r="C81">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="D81">
+        <v>3.89</v>
+      </c>
+      <c r="E81">
+        <v>2</v>
+      </c>
+      <c r="F81" t="s">
+        <v>25</v>
+      </c>
+      <c r="G81" t="s">
+        <v>156</v>
+      </c>
+      <c r="H81" t="s">
+        <v>23</v>
+      </c>
+      <c r="I81" s="2" t="d">
+        <v>2017-05-21</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>9</v>
+      </c>
+      <c r="B82" t="s">
+        <v>52</v>
+      </c>
+      <c r="C82">
+        <v>47</v>
+      </c>
+      <c r="D82">
+        <v>5.85</v>
+      </c>
+      <c r="E82">
+        <v>2</v>
+      </c>
+      <c r="F82" t="s">
+        <v>53</v>
+      </c>
+      <c r="G82" t="s">
+        <v>54</v>
+      </c>
+      <c r="H82" t="s">
+        <v>23</v>
+      </c>
+      <c r="I82" s="2" t="d">
+        <v>2013-05-23</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>9</v>
+      </c>
+      <c r="B83" t="s">
+        <v>97</v>
+      </c>
+      <c r="C83">
+        <v>50</v>
+      </c>
+      <c r="D83">
+        <v>4.58</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="F83" t="s">
+        <v>25</v>
+      </c>
+      <c r="G83" t="s">
+        <v>54</v>
+      </c>
+      <c r="H83" t="s">
+        <v>23</v>
+      </c>
+      <c r="I83" s="2" t="d">
+        <v>2013-05-26</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>9</v>
+      </c>
+      <c r="B84" t="s">
+        <v>140</v>
+      </c>
+      <c r="C84">
+        <v>23.5</v>
+      </c>
+      <c r="D84">
+        <v>5.41</v>
+      </c>
+      <c r="E84">
+        <v>2</v>
+      </c>
+      <c r="F84" t="s">
+        <v>11</v>
+      </c>
+      <c r="G84" t="s">
+        <v>15</v>
+      </c>
+      <c r="H84" t="s">
+        <v>23</v>
+      </c>
+      <c r="I84" s="2" t="d">
+        <v>2008-07-31</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>9</v>
+      </c>
+      <c r="B85">
+        <v>140</v>
+      </c>
+      <c r="C85">
+        <v>39.5</v>
+      </c>
+      <c r="D85">
+        <v>3.51</v>
+      </c>
+      <c r="E85">
+        <v>2</v>
+      </c>
+      <c r="F85" t="s">
+        <v>25</v>
+      </c>
+      <c r="G85" t="s">
+        <v>153</v>
+      </c>
+      <c r="H85" t="s">
+        <v>23</v>
+      </c>
+      <c r="I85" s="2" t="d">
+        <v>2014-05-06</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>9</v>
+      </c>
+      <c r="B86">
+        <v>185</v>
+      </c>
+      <c r="C86">
+        <v>34.4</v>
+      </c>
+      <c r="D86">
+        <v>5.33</v>
+      </c>
+      <c r="E86">
+        <v>2</v>
+      </c>
+      <c r="F86" t="s">
+        <v>25</v>
+      </c>
+      <c r="G86" t="s">
+        <v>152</v>
+      </c>
+      <c r="H86" t="s">
+        <v>23</v>
+      </c>
+      <c r="I86" s="2" t="d">
+        <v>2019-05-05</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>9</v>
+      </c>
+      <c r="B87" t="s">
+        <v>147</v>
+      </c>
+      <c r="C87">
+        <v>17.2</v>
+      </c>
+      <c r="D87">
+        <v>4.84</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="F87" t="s">
+        <v>55</v>
+      </c>
+      <c r="G87" t="s">
+        <v>152</v>
+      </c>
+      <c r="H87" t="s">
+        <v>23</v>
+      </c>
+      <c r="I87" s="2" t="d">
+        <v>2007-07-14</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>9</v>
+      </c>
+      <c r="B88">
+        <v>216</v>
+      </c>
+      <c r="C88">
+        <v>40.4</v>
+      </c>
+      <c r="D88">
+        <v>5.31</v>
+      </c>
+      <c r="E88">
+        <v>2</v>
+      </c>
+      <c r="F88" t="s">
+        <v>25</v>
+      </c>
+      <c r="G88" t="s">
+        <v>153</v>
+      </c>
+      <c r="H88" t="s">
+        <v>23</v>
+      </c>
+      <c r="I88" s="2" t="d">
+        <v>2016-06-16</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>9</v>
+      </c>
+      <c r="B89">
+        <v>181</v>
+      </c>
+      <c r="C89">
+        <v>46.3</v>
+      </c>
+      <c r="D89">
+        <v>3.89</v>
+      </c>
+      <c r="E89">
+        <v>1</v>
+      </c>
+      <c r="F89" t="s">
+        <v>25</v>
+      </c>
+      <c r="G89" t="s">
+        <v>42</v>
+      </c>
+      <c r="H89" t="s">
+        <v>159</v>
+      </c>
+      <c r="I89" s="2" t="d">
+        <v>2017-05-19</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>9</v>
+      </c>
+      <c r="B90" t="s">
+        <v>150</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90" t="s">
+        <v>151</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90" t="s">
+        <v>55</v>
+      </c>
+      <c r="G90" t="s">
+        <v>42</v>
+      </c>
+      <c r="H90" t="s">
+        <v>159</v>
+      </c>
+      <c r="I90" s="2" t="d">
+        <v>2017-05-12</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>9</v>
+      </c>
+      <c r="B91" t="s">
+        <v>59</v>
+      </c>
+      <c r="C91">
+        <v>50</v>
+      </c>
+      <c r="D91">
+        <v>5.38</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="F91" t="s">
+        <v>25</v>
+      </c>
+      <c r="G91" t="s">
+        <v>17</v>
+      </c>
+      <c r="H91" t="s">
+        <v>159</v>
+      </c>
+      <c r="I91" s="2" t="d">
+        <v>2013-09-03</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>9</v>
+      </c>
+      <c r="B92">
+        <v>198</v>
+      </c>
+      <c r="C92">
+        <v>43.1</v>
+      </c>
+      <c r="D92">
+        <v>4.58</v>
+      </c>
+      <c r="E92">
+        <v>1</v>
+      </c>
+      <c r="F92" t="s">
+        <v>25</v>
+      </c>
+      <c r="G92" t="s">
+        <v>17</v>
+      </c>
+      <c r="H92" t="s">
+        <v>159</v>
+      </c>
+      <c r="I92" s="2" t="d">
+        <v>2019-05-03</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>9</v>
+      </c>
+      <c r="B93" t="s">
+        <v>148</v>
+      </c>
+      <c r="C93">
+        <v>18</v>
+      </c>
+      <c r="D93">
+        <v>3.11</v>
+      </c>
+      <c r="E93">
+        <v>1</v>
+      </c>
+      <c r="F93" t="s">
+        <v>55</v>
+      </c>
+      <c r="G93" t="s">
+        <v>17</v>
+      </c>
+      <c r="H93" t="s">
+        <v>159</v>
+      </c>
+      <c r="I93" s="2" t="d">
+        <v>2015-05-08</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>9</v>
+      </c>
+      <c r="B94">
+        <v>82</v>
+      </c>
+      <c r="C94">
+        <v>23.4</v>
+      </c>
+      <c r="D94">
+        <v>3.46</v>
+      </c>
+      <c r="E94">
+        <v>2</v>
+      </c>
+      <c r="F94" t="s">
+        <v>25</v>
+      </c>
+      <c r="G94" t="s">
+        <v>54</v>
+      </c>
+      <c r="H94" t="s">
+        <v>159</v>
+      </c>
+      <c r="I94" s="2" t="d">
+        <v>2016-08-18</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>9</v>
+      </c>
+      <c r="B95" t="s">
+        <v>81</v>
+      </c>
+      <c r="C95">
+        <v>50</v>
+      </c>
+      <c r="D95">
+        <v>4.82</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+      <c r="F95" t="s">
+        <v>25</v>
+      </c>
+      <c r="G95" t="s">
+        <v>15</v>
+      </c>
+      <c r="H95" t="s">
+        <v>159</v>
+      </c>
+      <c r="I95" s="2" t="d">
+        <v>2014-09-12</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>9</v>
+      </c>
+      <c r="B96" t="s">
+        <v>100</v>
+      </c>
+      <c r="C96">
+        <v>44.2</v>
+      </c>
+      <c r="D96">
+        <v>5.07</v>
+      </c>
+      <c r="E96">
+        <v>2</v>
+      </c>
+      <c r="F96" t="s">
+        <v>11</v>
+      </c>
+      <c r="G96" t="s">
+        <v>15</v>
+      </c>
+      <c r="H96" t="s">
+        <v>159</v>
+      </c>
+      <c r="I96" s="2" t="d">
+        <v>2014-09-10</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>9</v>
+      </c>
+      <c r="B97" t="s">
+        <v>132</v>
+      </c>
+      <c r="C97">
+        <v>36.4</v>
+      </c>
+      <c r="D97">
+        <v>4.71</v>
+      </c>
+      <c r="E97">
+        <v>2</v>
+      </c>
+      <c r="F97" t="s">
+        <v>11</v>
+      </c>
+      <c r="G97" t="s">
+        <v>15</v>
+      </c>
+      <c r="H97" t="s">
+        <v>159</v>
+      </c>
+      <c r="I97" s="2" t="d">
+        <v>2014-09-08</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>9</v>
+      </c>
+      <c r="B98">
+        <v>241</v>
+      </c>
+      <c r="C98">
+        <v>45</v>
+      </c>
+      <c r="D98">
+        <v>5.35</v>
+      </c>
+      <c r="E98">
+        <v>2</v>
+      </c>
+      <c r="F98" t="s">
+        <v>25</v>
+      </c>
+      <c r="G98" t="s">
+        <v>153</v>
+      </c>
+      <c r="H98" t="s">
+        <v>159</v>
+      </c>
+      <c r="I98" s="2" t="d">
+        <v>2016-06-18</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>9</v>
+      </c>
+      <c r="B99" t="s">
+        <v>24</v>
+      </c>
+      <c r="C99">
+        <v>50</v>
+      </c>
+      <c r="D99">
+        <v>6.54</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+      <c r="F99" t="s">
+        <v>25</v>
+      </c>
+      <c r="G99" t="s">
+        <v>152</v>
+      </c>
+      <c r="H99" t="s">
+        <v>159</v>
+      </c>
+      <c r="I99" s="2" t="d">
+        <v>2019-05-11</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>9</v>
+      </c>
+      <c r="B100" t="s">
+        <v>28</v>
+      </c>
+      <c r="C100">
+        <v>50</v>
+      </c>
+      <c r="D100">
+        <v>6.4</v>
+      </c>
+      <c r="E100">
+        <v>1</v>
+      </c>
+      <c r="F100" t="s">
+        <v>25</v>
+      </c>
+      <c r="G100" t="s">
+        <v>15</v>
+      </c>
+      <c r="H100" t="s">
+        <v>29</v>
+      </c>
+      <c r="I100" s="2" t="d">
+        <v>2011-07-12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>9</v>
+      </c>
+      <c r="B101">
+        <v>304</v>
+      </c>
+      <c r="C101">
+        <v>47.3</v>
+      </c>
+      <c r="D101">
+        <v>6.4</v>
+      </c>
+      <c r="E101">
+        <v>2</v>
+      </c>
+      <c r="F101" t="s">
+        <v>25</v>
+      </c>
+      <c r="G101" t="s">
+        <v>39</v>
+      </c>
+      <c r="H101" t="s">
+        <v>160</v>
+      </c>
+      <c r="I101" s="2" t="d">
+        <v>2017-03-17</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>9</v>
+      </c>
+      <c r="B102" t="s">
+        <v>66</v>
+      </c>
+      <c r="C102">
+        <v>48.3</v>
+      </c>
+      <c r="D102">
+        <v>5.46</v>
+      </c>
+      <c r="E102">
+        <v>2</v>
+      </c>
+      <c r="F102" t="s">
+        <v>11</v>
+      </c>
+      <c r="G102" t="s">
+        <v>39</v>
+      </c>
+      <c r="H102" t="s">
+        <v>160</v>
+      </c>
+      <c r="I102" s="2" t="d">
+        <v>2017-03-19</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>9</v>
+      </c>
+      <c r="B103">
+        <v>262</v>
+      </c>
+      <c r="C103">
+        <v>46.5</v>
+      </c>
+      <c r="D103">
+        <v>5.59</v>
+      </c>
+      <c r="E103">
+        <v>2</v>
+      </c>
+      <c r="F103" t="s">
+        <v>25</v>
+      </c>
+      <c r="G103" t="s">
+        <v>39</v>
+      </c>
+      <c r="H103" t="s">
+        <v>160</v>
+      </c>
+      <c r="I103" s="2" t="d">
+        <v>2017-03-15</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>9</v>
+      </c>
+      <c r="B104">
+        <v>229</v>
+      </c>
+      <c r="C104">
+        <v>48.1</v>
+      </c>
+      <c r="D104">
+        <v>4.75</v>
+      </c>
+      <c r="E104">
+        <v>1</v>
+      </c>
+      <c r="F104" t="s">
+        <v>25</v>
+      </c>
+      <c r="G104" t="s">
+        <v>39</v>
+      </c>
+      <c r="H104" t="s">
+        <v>160</v>
+      </c>
+      <c r="I104" s="2" t="d">
+        <v>2017-03-24</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>9</v>
+      </c>
+      <c r="B105" t="s">
+        <v>101</v>
+      </c>
+      <c r="C105">
+        <v>46.5</v>
+      </c>
+      <c r="D105">
+        <v>4.78</v>
+      </c>
+      <c r="E105">
+        <v>2</v>
+      </c>
+      <c r="F105" t="s">
+        <v>11</v>
+      </c>
+      <c r="G105" t="s">
+        <v>39</v>
+      </c>
+      <c r="H105" t="s">
+        <v>160</v>
+      </c>
+      <c r="I105" s="2" t="d">
+        <v>2017-03-22</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>9</v>
+      </c>
+      <c r="B106">
+        <v>259</v>
+      </c>
+      <c r="C106">
+        <v>49</v>
+      </c>
+      <c r="D106">
+        <v>5.28</v>
+      </c>
+      <c r="E106">
+        <v>1</v>
+      </c>
+      <c r="F106" t="s">
+        <v>25</v>
+      </c>
+      <c r="G106" t="s">
+        <v>70</v>
+      </c>
+      <c r="H106" t="s">
+        <v>71</v>
+      </c>
+      <c r="I106" s="2" t="d">
+        <v>2015-03-10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>9</v>
+      </c>
+      <c r="B107" t="s">
+        <v>116</v>
+      </c>
+      <c r="C107">
+        <v>50</v>
+      </c>
+      <c r="D107">
+        <v>4.18</v>
+      </c>
+      <c r="E107">
+        <v>1</v>
+      </c>
+      <c r="F107" t="s">
+        <v>25</v>
+      </c>
+      <c r="G107" t="s">
+        <v>39</v>
+      </c>
+      <c r="H107" t="s">
+        <v>32</v>
+      </c>
+      <c r="I107" s="2" t="d">
+        <v>2018-03-23</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>9</v>
+      </c>
+      <c r="B108" t="s">
+        <v>90</v>
+      </c>
+      <c r="C108">
+        <v>49.1</v>
+      </c>
+      <c r="D108">
+        <v>4.82</v>
+      </c>
+      <c r="E108">
+        <v>2</v>
+      </c>
+      <c r="F108" t="s">
+        <v>11</v>
+      </c>
+      <c r="G108" t="s">
+        <v>91</v>
+      </c>
+      <c r="H108" t="s">
+        <v>32</v>
+      </c>
+      <c r="I108" s="2" t="d">
+        <v>2018-03-06</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>9</v>
+      </c>
+      <c r="B109" t="s">
+        <v>57</v>
+      </c>
+      <c r="C109">
+        <v>50</v>
+      </c>
+      <c r="D109">
+        <v>5.42</v>
+      </c>
+      <c r="E109">
+        <v>1</v>
+      </c>
+      <c r="F109" t="s">
+        <v>11</v>
+      </c>
+      <c r="G109" t="s">
+        <v>15</v>
+      </c>
+      <c r="H109" t="s">
+        <v>32</v>
+      </c>
+      <c r="I109" s="2" t="d">
+        <v>2018-03-18</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>9</v>
+      </c>
+      <c r="B110" t="s">
+        <v>30</v>
+      </c>
+      <c r="C110">
+        <v>44</v>
+      </c>
+      <c r="D110">
+        <v>7.11</v>
+      </c>
+      <c r="E110">
+        <v>1</v>
+      </c>
+      <c r="F110" t="s">
+        <v>11</v>
+      </c>
+      <c r="G110" t="s">
+        <v>31</v>
+      </c>
+      <c r="H110" t="s">
+        <v>32</v>
+      </c>
+      <c r="I110" s="2" t="d">
+        <v>2018-03-12</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>9</v>
+      </c>
+      <c r="B111">
+        <v>205</v>
+      </c>
+      <c r="C111">
+        <v>46.2</v>
+      </c>
+      <c r="D111">
+        <v>4.42</v>
+      </c>
+      <c r="E111">
+        <v>2</v>
+      </c>
+      <c r="F111" t="s">
+        <v>25</v>
+      </c>
+      <c r="G111" t="s">
+        <v>152</v>
+      </c>
+      <c r="H111" t="s">
+        <v>32</v>
+      </c>
+      <c r="I111" s="2" t="d">
+        <v>2018-03-10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>9</v>
+      </c>
+      <c r="B112" t="s">
+        <v>63</v>
+      </c>
+      <c r="C112">
+        <v>50</v>
+      </c>
+      <c r="D112">
+        <v>5.36</v>
+      </c>
+      <c r="E112">
+        <v>1</v>
+      </c>
+      <c r="F112" t="s">
+        <v>25</v>
+      </c>
+      <c r="G112" t="s">
+        <v>12</v>
+      </c>
+      <c r="H112" t="s">
+        <v>32</v>
+      </c>
+      <c r="I112" s="2" t="d">
+        <v>2015-10-11</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>9</v>
+      </c>
+      <c r="B113">
+        <v>244</v>
+      </c>
+      <c r="C113">
+        <v>49.4</v>
+      </c>
+      <c r="D113">
+        <v>4.91</v>
+      </c>
+      <c r="E113">
+        <v>1</v>
+      </c>
+      <c r="F113" t="s">
+        <v>11</v>
+      </c>
+      <c r="G113" t="s">
+        <v>12</v>
+      </c>
+      <c r="H113" t="s">
+        <v>32</v>
+      </c>
+      <c r="I113" s="2" t="d">
+        <v>2010-09-30</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>9</v>
+      </c>
+      <c r="B114" t="s">
+        <v>83</v>
+      </c>
+      <c r="C114">
+        <v>50</v>
+      </c>
+      <c r="D114">
+        <v>4.76</v>
+      </c>
+      <c r="E114">
+        <v>1</v>
+      </c>
+      <c r="F114" t="s">
+        <v>25</v>
+      </c>
+      <c r="G114" t="s">
+        <v>12</v>
+      </c>
+      <c r="H114" t="s">
+        <v>32</v>
+      </c>
+      <c r="I114" s="2" t="d">
+        <v>2010-09-28</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>9</v>
+      </c>
+      <c r="B115" t="s">
+        <v>107</v>
+      </c>
+      <c r="C115">
+        <v>50</v>
+      </c>
+      <c r="D115">
+        <v>4.38</v>
+      </c>
+      <c r="E115">
+        <v>1</v>
+      </c>
+      <c r="F115" t="s">
+        <v>25</v>
+      </c>
+      <c r="G115" t="s">
+        <v>12</v>
+      </c>
+      <c r="H115" t="s">
+        <v>32</v>
+      </c>
+      <c r="I115" s="2" t="d">
+        <v>2015-10-09</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>9</v>
+      </c>
+      <c r="B116">
+        <v>200</v>
+      </c>
+      <c r="C116">
+        <v>47.3</v>
+      </c>
+      <c r="D116">
+        <v>4.21</v>
+      </c>
+      <c r="E116">
+        <v>1</v>
+      </c>
+      <c r="F116" t="s">
+        <v>25</v>
+      </c>
+      <c r="G116" t="s">
+        <v>12</v>
+      </c>
+      <c r="H116" t="s">
+        <v>32</v>
+      </c>
+      <c r="I116" s="2" t="d">
+        <v>2010-09-26</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>9</v>
+      </c>
+      <c r="B117" t="s">
+        <v>123</v>
+      </c>
+      <c r="C117">
+        <v>46.5</v>
+      </c>
+      <c r="D117">
+        <v>4.03</v>
+      </c>
+      <c r="E117">
+        <v>2</v>
+      </c>
+      <c r="F117" t="s">
+        <v>11</v>
+      </c>
+      <c r="G117" t="s">
+        <v>12</v>
+      </c>
+      <c r="H117" t="s">
+        <v>32</v>
+      </c>
+      <c r="I117" s="2" t="d">
+        <v>2015-10-13</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>9</v>
+      </c>
+      <c r="B118">
+        <v>104</v>
+      </c>
+      <c r="C118">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="D118">
+        <v>3.02</v>
+      </c>
+      <c r="E118">
+        <v>2</v>
+      </c>
+      <c r="F118" t="s">
+        <v>25</v>
+      </c>
+      <c r="G118" t="s">
+        <v>12</v>
+      </c>
+      <c r="H118" t="s">
+        <v>32</v>
+      </c>
+      <c r="I118" s="2" t="d">
+        <v>2018-03-16</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>9</v>
+      </c>
+      <c r="B119" t="s">
+        <v>10</v>
+      </c>
+      <c r="C119">
+        <v>50</v>
+      </c>
+      <c r="D119">
+        <v>6.62</v>
+      </c>
+      <c r="E119">
+        <v>1</v>
+      </c>
+      <c r="F119" t="s">
+        <v>11</v>
+      </c>
+      <c r="G119" t="s">
+        <v>12</v>
+      </c>
+      <c r="H119" t="s">
+        <v>13</v>
+      </c>
+      <c r="I119" s="2" t="d">
+        <v>2015-03-07</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>9</v>
+      </c>
+      <c r="B120" t="s">
+        <v>14</v>
+      </c>
+      <c r="C120">
+        <v>50</v>
+      </c>
+      <c r="D120">
+        <v>6.62</v>
+      </c>
+      <c r="E120">
+        <v>1</v>
+      </c>
+      <c r="F120" t="s">
+        <v>11</v>
+      </c>
+      <c r="G120" t="s">
+        <v>15</v>
+      </c>
+      <c r="H120" t="s">
+        <v>161</v>
+      </c>
+      <c r="I120" s="2" t="d">
+        <v>2018-01-18</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>9</v>
+      </c>
+      <c r="B121" t="s">
+        <v>102</v>
+      </c>
+      <c r="C121">
+        <v>34.5</v>
+      </c>
+      <c r="D121">
+        <v>6.4</v>
+      </c>
+      <c r="E121">
+        <v>2</v>
+      </c>
+      <c r="F121" t="s">
+        <v>11</v>
+      </c>
+      <c r="G121" t="s">
+        <v>15</v>
+      </c>
+      <c r="H121" t="s">
+        <v>161</v>
+      </c>
+      <c r="I121" s="2" t="d">
+        <v>2018-01-16</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>9</v>
+      </c>
+      <c r="B122" t="s">
+        <v>150</v>
+      </c>
+      <c r="C122">
+        <v>0</v>
+      </c>
+      <c r="D122" t="s">
+        <v>151</v>
+      </c>
+      <c r="E122">
+        <v>0</v>
+      </c>
+      <c r="F122" t="s">
+        <v>55</v>
+      </c>
+      <c r="G122" t="s">
+        <v>15</v>
+      </c>
+      <c r="H122" t="s">
+        <v>161</v>
+      </c>
+      <c r="I122" s="2" t="d">
+        <v>2015-01-19</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>9</v>
+      </c>
+      <c r="B123" t="s">
+        <v>40</v>
+      </c>
+      <c r="C123">
+        <v>50</v>
+      </c>
+      <c r="D123">
+        <v>6.02</v>
+      </c>
+      <c r="E123">
+        <v>1</v>
+      </c>
+      <c r="F123" t="s">
+        <v>11</v>
+      </c>
+      <c r="G123" t="s">
+        <v>31</v>
+      </c>
+      <c r="H123" t="s">
+        <v>161</v>
+      </c>
+      <c r="I123" s="2" t="d">
+        <v>2018-01-13</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>9</v>
+      </c>
+      <c r="B124">
+        <v>270</v>
+      </c>
+      <c r="C124">
+        <v>49.3</v>
+      </c>
+      <c r="D124">
+        <v>5.45</v>
+      </c>
+      <c r="E124">
+        <v>1</v>
+      </c>
+      <c r="F124" t="s">
+        <v>11</v>
+      </c>
+      <c r="G124" t="s">
+        <v>31</v>
+      </c>
+      <c r="H124" t="s">
+        <v>161</v>
+      </c>
+      <c r="I124" s="2" t="d">
+        <v>2017-03-02</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>9</v>
+      </c>
+      <c r="B125" t="s">
+        <v>98</v>
+      </c>
+      <c r="C125">
+        <v>49.2</v>
+      </c>
+      <c r="D125">
+        <v>4.58</v>
+      </c>
+      <c r="E125">
+        <v>2</v>
+      </c>
+      <c r="F125" t="s">
+        <v>11</v>
+      </c>
+      <c r="G125" t="s">
+        <v>31</v>
+      </c>
+      <c r="H125" t="s">
+        <v>161</v>
+      </c>
+      <c r="I125" s="2" t="d">
+        <v>2018-01-11</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>9</v>
+      </c>
+      <c r="B126" t="s">
+        <v>118</v>
+      </c>
+      <c r="C126">
+        <v>41.5</v>
+      </c>
+      <c r="D126">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="E126">
+        <v>2</v>
+      </c>
+      <c r="F126" t="s">
+        <v>11</v>
+      </c>
+      <c r="G126" t="s">
+        <v>31</v>
+      </c>
+      <c r="H126" t="s">
+        <v>161</v>
+      </c>
+      <c r="I126" s="2" t="d">
+        <v>2017-03-04</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>9</v>
+      </c>
+      <c r="B127" t="s">
+        <v>139</v>
+      </c>
+      <c r="C127">
+        <v>41.4</v>
+      </c>
+      <c r="D127">
+        <v>3.19</v>
+      </c>
+      <c r="E127">
+        <v>2</v>
+      </c>
+      <c r="F127" t="s">
+        <v>11</v>
+      </c>
+      <c r="G127" t="s">
+        <v>54</v>
+      </c>
+      <c r="H127" t="s">
+        <v>105</v>
+      </c>
+      <c r="I127" s="2" t="d">
+        <v>2007-03-17</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>9</v>
+      </c>
+      <c r="B128">
+        <v>219</v>
+      </c>
+      <c r="C128">
+        <v>50</v>
+      </c>
+      <c r="D128">
+        <v>4.38</v>
+      </c>
+      <c r="E128">
+        <v>1</v>
+      </c>
+      <c r="F128" t="s">
+        <v>25</v>
+      </c>
+      <c r="G128" t="s">
+        <v>152</v>
+      </c>
+      <c r="H128" t="s">
+        <v>105</v>
+      </c>
+      <c r="I128" s="2" t="d">
+        <v>2010-04-15</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>9</v>
+      </c>
+      <c r="B129">
+        <v>202</v>
+      </c>
+      <c r="C129">
+        <v>49.2</v>
+      </c>
+      <c r="D129">
+        <v>4.09</v>
+      </c>
+      <c r="E129">
+        <v>1</v>
+      </c>
+      <c r="F129" t="s">
+        <v>25</v>
+      </c>
+      <c r="G129" t="s">
+        <v>152</v>
+      </c>
+      <c r="H129" t="s">
+        <v>105</v>
+      </c>
+      <c r="I129" s="2" t="d">
+        <v>2014-02-23</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>9</v>
+      </c>
+      <c r="B130" t="s">
+        <v>127</v>
+      </c>
+      <c r="C130">
+        <v>48</v>
+      </c>
+      <c r="D130">
+        <v>3.81</v>
+      </c>
+      <c r="E130">
+        <v>1</v>
+      </c>
+      <c r="F130" t="s">
+        <v>25</v>
+      </c>
+      <c r="G130" t="s">
+        <v>152</v>
+      </c>
+      <c r="H130" t="s">
+        <v>105</v>
+      </c>
+      <c r="I130" s="2" t="d">
+        <v>2007-03-23</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>9</v>
+      </c>
+      <c r="B131" t="s">
+        <v>104</v>
+      </c>
+      <c r="C131">
+        <v>50</v>
+      </c>
+      <c r="D131">
+        <v>4.42</v>
+      </c>
+      <c r="E131">
+        <v>1</v>
+      </c>
+      <c r="F131" t="s">
+        <v>53</v>
+      </c>
+      <c r="G131" t="s">
+        <v>12</v>
+      </c>
+      <c r="H131" t="s">
+        <v>105</v>
+      </c>
+      <c r="I131" s="2" t="d">
+        <v>2007-03-15</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>9</v>
+      </c>
+      <c r="B132" t="s">
+        <v>34</v>
+      </c>
+      <c r="C132">
+        <v>47.4</v>
+      </c>
+      <c r="D132">
+        <v>6.44</v>
+      </c>
+      <c r="E132">
+        <v>2</v>
+      </c>
+      <c r="F132" t="s">
+        <v>11</v>
+      </c>
+      <c r="G132" t="s">
+        <v>35</v>
+      </c>
+      <c r="H132" t="s">
+        <v>36</v>
+      </c>
+      <c r="I132" s="2" t="d">
+        <v>2011-03-18</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>9</v>
+      </c>
+      <c r="B133">
+        <v>141</v>
+      </c>
+      <c r="C133">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="D133">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="E133">
+        <v>2</v>
+      </c>
+      <c r="F133" t="s">
+        <v>25</v>
+      </c>
+      <c r="G133" t="s">
+        <v>155</v>
+      </c>
+      <c r="H133" t="s">
+        <v>36</v>
+      </c>
+      <c r="I133" s="2" t="d">
+        <v>2011-03-15</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>9</v>
+      </c>
+      <c r="B134">
+        <v>243</v>
+      </c>
+      <c r="C134">
+        <v>46.1</v>
+      </c>
+      <c r="D134">
+        <v>5.26</v>
+      </c>
+      <c r="E134">
+        <v>2</v>
+      </c>
+      <c r="F134" t="s">
+        <v>25</v>
+      </c>
+      <c r="G134" t="s">
+        <v>17</v>
+      </c>
+      <c r="H134" t="s">
+        <v>79</v>
+      </c>
+      <c r="I134" s="2" t="d">
+        <v>2017-05-07</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>9</v>
+      </c>
+      <c r="B135">
+        <v>231</v>
+      </c>
+      <c r="C135">
+        <v>49</v>
+      </c>
+      <c r="D135">
+        <v>4.71</v>
+      </c>
+      <c r="E135">
+        <v>2</v>
+      </c>
+      <c r="F135" t="s">
+        <v>25</v>
+      </c>
+      <c r="G135" t="s">
+        <v>152</v>
+      </c>
+      <c r="H135" t="s">
+        <v>96</v>
+      </c>
+      <c r="I135" s="2" t="d">
+        <v>2011-03-11</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>9</v>
+      </c>
+      <c r="B136" t="s">
+        <v>85</v>
+      </c>
+      <c r="C136">
+        <v>50</v>
+      </c>
+      <c r="D136">
+        <v>4.74</v>
+      </c>
+      <c r="E136">
+        <v>1</v>
+      </c>
+      <c r="F136" t="s">
+        <v>11</v>
+      </c>
+      <c r="G136" t="s">
+        <v>44</v>
+      </c>
+      <c r="H136" t="s">
+        <v>87</v>
+      </c>
+      <c r="I136" s="2" t="d">
+        <v>2012-02-20</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>9</v>
+      </c>
+      <c r="B137">
+        <v>200</v>
+      </c>
+      <c r="C137">
+        <v>47.3</v>
+      </c>
+      <c r="D137">
+        <v>4.21</v>
+      </c>
+      <c r="E137">
+        <v>1</v>
+      </c>
+      <c r="F137" t="s">
+        <v>25</v>
+      </c>
+      <c r="G137" t="s">
+        <v>44</v>
+      </c>
+      <c r="H137" t="s">
+        <v>87</v>
+      </c>
+      <c r="I137" s="2" t="d">
+        <v>2012-02-18</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>9</v>
+      </c>
+      <c r="B138" t="s">
+        <v>43</v>
+      </c>
+      <c r="C138">
+        <v>47</v>
+      </c>
+      <c r="D138">
+        <v>6.06</v>
+      </c>
+      <c r="E138">
+        <v>1</v>
+      </c>
+      <c r="F138" t="s">
+        <v>11</v>
+      </c>
+      <c r="G138" t="s">
+        <v>44</v>
+      </c>
+      <c r="H138" t="s">
+        <v>162</v>
+      </c>
+      <c r="I138" s="2" t="d">
+        <v>2008-10-18</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>9</v>
+      </c>
+      <c r="B139" t="s">
+        <v>75</v>
+      </c>
+      <c r="C139">
+        <v>46</v>
+      </c>
+      <c r="D139">
+        <v>5.52</v>
+      </c>
+      <c r="E139">
+        <v>2</v>
+      </c>
+      <c r="F139" t="s">
+        <v>25</v>
+      </c>
+      <c r="G139" t="s">
+        <v>35</v>
+      </c>
+      <c r="H139" t="s">
+        <v>162</v>
+      </c>
+      <c r="I139" s="2" t="d">
+        <v>2007-02-05</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>9</v>
+      </c>
+      <c r="B140" t="s">
+        <v>46</v>
+      </c>
+      <c r="C140">
+        <v>50</v>
+      </c>
+      <c r="D140">
+        <v>5.6</v>
+      </c>
+      <c r="E140">
+        <v>1</v>
+      </c>
+      <c r="F140" t="s">
+        <v>25</v>
+      </c>
+      <c r="G140" t="s">
+        <v>15</v>
+      </c>
+      <c r="H140" t="s">
+        <v>162</v>
+      </c>
+      <c r="I140" s="2" t="d">
+        <v>2007-01-30</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>9</v>
+      </c>
+      <c r="B141">
+        <v>147</v>
+      </c>
+      <c r="C141">
+        <v>46.1</v>
+      </c>
+      <c r="D141">
+        <v>3.18</v>
+      </c>
+      <c r="E141">
+        <v>2</v>
+      </c>
+      <c r="F141" t="s">
+        <v>25</v>
+      </c>
+      <c r="G141" t="s">
+        <v>12</v>
+      </c>
+      <c r="H141" t="s">
+        <v>162</v>
+      </c>
+      <c r="I141" s="2" t="d">
+        <v>2008-10-17</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>9</v>
+      </c>
+      <c r="B142" t="s">
+        <v>49</v>
+      </c>
+      <c r="C142">
+        <v>48.4</v>
+      </c>
+      <c r="D142">
+        <v>5.67</v>
+      </c>
+      <c r="E142">
+        <v>2</v>
+      </c>
+      <c r="F142" t="s">
+        <v>11</v>
+      </c>
+      <c r="G142" t="s">
+        <v>50</v>
+      </c>
+      <c r="H142" t="s">
+        <v>163</v>
+      </c>
+      <c r="I142" s="2" t="d">
+        <v>2007-01-31</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>9</v>
+      </c>
+      <c r="B143" t="s">
+        <v>33</v>
+      </c>
+      <c r="C143">
+        <v>50</v>
+      </c>
+      <c r="D143">
+        <v>6.16</v>
+      </c>
+      <c r="E143">
+        <v>1</v>
+      </c>
+      <c r="F143" t="s">
+        <v>25</v>
+      </c>
+      <c r="G143" t="s">
+        <v>22</v>
+      </c>
+      <c r="H143" t="s">
+        <v>163</v>
+      </c>
+      <c r="I143" s="2" t="d">
+        <v>2007-02-04</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>9</v>
+      </c>
+      <c r="B144" t="s">
+        <v>45</v>
+      </c>
+      <c r="C144">
+        <v>50</v>
+      </c>
+      <c r="D144">
+        <v>5.68</v>
+      </c>
+      <c r="E144">
+        <v>1</v>
+      </c>
+      <c r="F144" t="s">
+        <v>25</v>
+      </c>
+      <c r="G144" t="s">
+        <v>44</v>
+      </c>
+      <c r="H144" t="s">
+        <v>164</v>
+      </c>
+      <c r="I144" s="2" t="d">
+        <v>2007-02-02</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>9</v>
+      </c>
+      <c r="B145" t="s">
+        <v>37</v>
+      </c>
+      <c r="C145">
+        <v>45.5</v>
+      </c>
+      <c r="D145">
+        <v>6.69</v>
+      </c>
+      <c r="E145">
+        <v>2</v>
+      </c>
+      <c r="F145" t="s">
+        <v>11</v>
+      </c>
+      <c r="G145" t="s">
+        <v>152</v>
+      </c>
+      <c r="H145" t="s">
+        <v>38</v>
+      </c>
+      <c r="I145" s="2" t="d">
+        <v>2015-02-16</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>9</v>
+      </c>
+      <c r="B146">
+        <v>218</v>
+      </c>
+      <c r="C146">
+        <v>48.1</v>
+      </c>
+      <c r="D146">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="E146">
+        <v>2</v>
+      </c>
+      <c r="F146" t="s">
+        <v>25</v>
+      </c>
+      <c r="G146" t="s">
+        <v>17</v>
+      </c>
+      <c r="H146" t="s">
+        <v>109</v>
+      </c>
+      <c r="I146" s="2" t="d">
+        <v>2007-03-30</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>9</v>
+      </c>
+      <c r="B147">
+        <v>134</v>
+      </c>
+      <c r="C147">
+        <v>37.4</v>
+      </c>
+      <c r="D147">
+        <v>3.55</v>
+      </c>
+      <c r="E147">
+        <v>2</v>
+      </c>
+      <c r="F147" t="s">
+        <v>25</v>
+      </c>
+      <c r="G147" t="s">
+        <v>156</v>
+      </c>
+      <c r="H147" t="s">
+        <v>109</v>
+      </c>
+      <c r="I147" s="2" t="d">
+        <v>2007-04-09</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>9</v>
+      </c>
+      <c r="B148" t="s">
+        <v>136</v>
+      </c>
+      <c r="C148">
+        <v>35</v>
+      </c>
+      <c r="D148">
+        <v>4.34</v>
+      </c>
+      <c r="E148">
+        <v>1</v>
+      </c>
+      <c r="F148" t="s">
+        <v>25</v>
+      </c>
+      <c r="G148" t="s">
+        <v>155</v>
+      </c>
+      <c r="H148" t="s">
+        <v>109</v>
+      </c>
+      <c r="I148" s="2" t="d">
+        <v>2007-04-03</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>9</v>
+      </c>
+      <c r="B149" t="s">
+        <v>85</v>
+      </c>
+      <c r="C149">
+        <v>50</v>
+      </c>
+      <c r="D149">
+        <v>4.74</v>
+      </c>
+      <c r="E149">
+        <v>1</v>
+      </c>
+      <c r="F149" t="s">
+        <v>11</v>
+      </c>
+      <c r="G149" t="s">
+        <v>39</v>
+      </c>
+      <c r="H149" t="s">
+        <v>86</v>
+      </c>
+      <c r="I149" s="2" t="d">
+        <v>2010-07-03</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>9</v>
+      </c>
+      <c r="B150" t="s">
+        <v>134</v>
+      </c>
+      <c r="C150">
+        <v>39.5</v>
+      </c>
+      <c r="D150">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="E150">
+        <v>2</v>
+      </c>
+      <c r="F150" t="s">
+        <v>11</v>
+      </c>
+      <c r="G150" t="s">
+        <v>44</v>
+      </c>
+      <c r="H150" t="s">
+        <v>86</v>
+      </c>
+      <c r="I150" s="2" t="d">
+        <v>2010-07-01</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>9</v>
+      </c>
+      <c r="B151" t="s">
+        <v>57</v>
+      </c>
+      <c r="C151">
+        <v>50</v>
+      </c>
+      <c r="D151">
+        <v>5.42</v>
+      </c>
+      <c r="E151">
+        <v>1</v>
+      </c>
+      <c r="F151" t="s">
+        <v>11</v>
+      </c>
+      <c r="G151" t="s">
+        <v>39</v>
+      </c>
+      <c r="H151" t="s">
+        <v>58</v>
+      </c>
+      <c r="I151" s="2" t="d">
+        <v>2017-12-07</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>9</v>
+      </c>
+      <c r="B152" t="s">
+        <v>130</v>
+      </c>
+      <c r="C152">
+        <v>38</v>
+      </c>
+      <c r="D152">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="E152">
+        <v>2</v>
+      </c>
+      <c r="F152" t="s">
+        <v>11</v>
+      </c>
+      <c r="G152" t="s">
+        <v>39</v>
+      </c>
+      <c r="H152" t="s">
+        <v>58</v>
+      </c>
+      <c r="I152" s="2" t="d">
+        <v>2017-12-10</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>9</v>
+      </c>
+      <c r="B153">
+        <v>100</v>
+      </c>
+      <c r="C153">
+        <v>31.4</v>
+      </c>
+      <c r="D153">
+        <v>3.15</v>
+      </c>
+      <c r="E153">
+        <v>2</v>
+      </c>
+      <c r="F153" t="s">
+        <v>25</v>
+      </c>
+      <c r="G153" t="s">
+        <v>39</v>
+      </c>
+      <c r="H153" t="s">
+        <v>58</v>
+      </c>
+      <c r="I153" s="2" t="d">
+        <v>2017-12-05</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>9</v>
+      </c>
+      <c r="B154" t="s">
+        <v>19</v>
+      </c>
+      <c r="C154">
+        <v>49.5</v>
+      </c>
+      <c r="D154">
+        <v>6.6</v>
+      </c>
+      <c r="E154">
+        <v>2</v>
+      </c>
+      <c r="F154" t="s">
+        <v>11</v>
+      </c>
+      <c r="G154" t="s">
+        <v>17</v>
+      </c>
+      <c r="H154" t="s">
+        <v>20</v>
+      </c>
+      <c r="I154" s="2" t="d">
+        <v>2020-08-04</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>9</v>
+      </c>
+      <c r="B155" t="s">
+        <v>112</v>
+      </c>
+      <c r="C155">
+        <v>50</v>
+      </c>
+      <c r="D155">
+        <v>4.24</v>
+      </c>
+      <c r="E155">
+        <v>1</v>
+      </c>
+      <c r="F155" t="s">
+        <v>25</v>
+      </c>
+      <c r="G155" t="s">
+        <v>17</v>
+      </c>
+      <c r="H155" t="s">
+        <v>20</v>
+      </c>
+      <c r="I155" s="2" t="d">
+        <v>2020-08-01</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>9</v>
+      </c>
+      <c r="B156">
+        <v>172</v>
+      </c>
+      <c r="C156">
+        <v>44.4</v>
+      </c>
+      <c r="D156">
+        <v>3.85</v>
+      </c>
+      <c r="E156">
+        <v>1</v>
+      </c>
+      <c r="F156" t="s">
+        <v>25</v>
+      </c>
+      <c r="G156" t="s">
+        <v>17</v>
+      </c>
+      <c r="H156" t="s">
+        <v>20</v>
+      </c>
+      <c r="I156" s="2" t="d">
+        <v>2020-07-30</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>9</v>
+      </c>
+      <c r="B157">
+        <v>203</v>
+      </c>
+      <c r="C157">
+        <v>49.1</v>
+      </c>
+      <c r="D157">
+        <v>4.12</v>
+      </c>
+      <c r="E157">
+        <v>1</v>
+      </c>
+      <c r="F157" t="s">
+        <v>25</v>
+      </c>
+      <c r="G157" t="s">
+        <v>152</v>
+      </c>
+      <c r="H157" t="s">
+        <v>119</v>
+      </c>
+      <c r="I157" s="2" t="d">
+        <v>2020-01-12</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>9</v>
+      </c>
+      <c r="B158">
+        <v>77</v>
+      </c>
+      <c r="C158">
+        <v>27.4</v>
+      </c>
+      <c r="D158">
+        <v>2.78</v>
+      </c>
+      <c r="E158">
+        <v>1</v>
+      </c>
+      <c r="F158" t="s">
+        <v>25</v>
+      </c>
+      <c r="G158" t="s">
+        <v>153</v>
+      </c>
+      <c r="H158" t="s">
+        <v>154</v>
+      </c>
+      <c r="I158" s="2" t="d">
+        <v>2007-04-18</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>9</v>
+      </c>
+      <c r="B159" t="s">
+        <v>143</v>
+      </c>
+      <c r="C159">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="D159">
+        <v>3.49</v>
+      </c>
+      <c r="E159">
+        <v>2</v>
+      </c>
+      <c r="F159" t="s">
+        <v>11</v>
+      </c>
+      <c r="G159" t="s">
+        <v>15</v>
+      </c>
+      <c r="H159" t="s">
+        <v>165</v>
+      </c>
+      <c r="I159" s="2" t="d">
+        <v>2010-07-05</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>9</v>
+      </c>
+      <c r="B160" t="s">
+        <v>26</v>
+      </c>
+      <c r="C160">
+        <v>50</v>
+      </c>
+      <c r="D160">
+        <v>6.5</v>
+      </c>
+      <c r="E160">
+        <v>1</v>
+      </c>
+      <c r="F160" t="s">
+        <v>11</v>
+      </c>
+      <c r="G160" t="s">
+        <v>22</v>
+      </c>
+      <c r="H160" t="s">
+        <v>27</v>
+      </c>
+      <c r="I160" s="2" t="d">
+        <v>2010-09-07</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>9</v>
+      </c>
+      <c r="B161" t="s">
+        <v>131</v>
+      </c>
+      <c r="C161">
+        <v>35</v>
+      </c>
+      <c r="D161">
+        <v>5</v>
+      </c>
+      <c r="E161">
+        <v>1</v>
+      </c>
+      <c r="F161" t="s">
+        <v>25</v>
+      </c>
+      <c r="G161" t="s">
+        <v>22</v>
+      </c>
+      <c r="H161" t="s">
+        <v>27</v>
+      </c>
+      <c r="I161" s="2" t="d">
+        <v>2010-09-06</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I162" s="2"/>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I163" s="2"/>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I164" s="2"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I164">
+    <sortCondition ref="H2:H164"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>